<commit_message>
Update Tasklist after testing with KX
</commit_message>
<xml_diff>
--- a/Tasklist deadline Monday 31 Oct 12 pm/Sprint2 bug fixes.xlsx
+++ b/Tasklist deadline Monday 31 Oct 12 pm/Sprint2 bug fixes.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP-GIT\Ulink\Tasklist deadline Monday 31 Oct 12 pm\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27080" windowHeight="17520"/>
   </bookViews>
@@ -15,18 +20,18 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="97">
   <si>
     <t>DEADLINE: 31 Oct 2016 – Monday before 12 PM</t>
   </si>
@@ -311,9 +316,6 @@
   </si>
   <si>
     <t>Client Module – Client Summary Page</t>
-  </si>
-  <si>
-    <t>Refer to process 1 and process 2</t>
   </si>
   <si>
     <r>
@@ -423,6 +425,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>(Auto-populated)</t>
@@ -437,11 +440,32 @@
   <si>
     <t>yes but havent integrate w sean to test</t>
   </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Fail(checkbox)</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Refer to process 1 and process 2(to be done in interation 5)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,6 +528,7 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -737,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -797,38 +822,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -879,16 +919,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>448373</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>672170</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>126272</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>128185</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>549235</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>1905000</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>193260</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>285625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -912,8 +952,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8735123" y="54043920"/>
-          <a:ext cx="1910612" cy="1232830"/>
+          <a:off x="13700547" y="10619489"/>
+          <a:ext cx="4999742" cy="4271136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -921,7 +961,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -934,16 +974,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>588625</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266883</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>35162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>246152</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>1901699</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>496957</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>376482</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -967,8 +1007,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6689687" y="54110563"/>
-          <a:ext cx="1882813" cy="1313074"/>
+          <a:off x="8291811" y="10526466"/>
+          <a:ext cx="5162827" cy="4832335"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -976,7 +1016,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -989,16 +1029,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>163513</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>469348</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>154309</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>158749</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>31754</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>156450</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>184057</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1013,8 +1053,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1288255" y="85521008"/>
-          <a:ext cx="4059240" cy="6635749"/>
+          <a:off x="12836974" y="17972191"/>
+          <a:ext cx="5183371" cy="7702826"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1025,16 +1065,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>598188</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>344649</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>158750</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>158749</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>140344</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>57517</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1049,8 +1089,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="7921624" y="85740875"/>
-          <a:ext cx="3937000" cy="6191250"/>
+          <a:off x="9881383" y="14068701"/>
+          <a:ext cx="3808158" cy="6324692"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1351,7 +1391,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1359,25 +1399,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="38.36328125" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="21" thickBot="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1385,53 +1425,53 @@
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="22"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="E3" s="34"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="16" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29.25" customHeight="1">
-      <c r="A5" s="23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="26"/>
-      <c r="E5" s="18"/>
-    </row>
-    <row r="6" spans="1:5" ht="21" customHeight="1" thickBot="1">
+      <c r="E5" s="30"/>
+    </row>
+    <row r="6" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1">
+      <c r="D6" s="27"/>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1442,11 +1482,13 @@
         <v>11</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1">
+        <v>83</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1454,14 +1496,16 @@
         <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1">
+        <v>83</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1474,7 +1518,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:5" ht="29" thickBot="1">
+    <row r="10" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1487,93 +1531,97 @@
       <c r="D10" s="11"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:5" ht="42">
-      <c r="A11" s="23" t="s">
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="24" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="18"/>
-    </row>
-    <row r="12" spans="1:5" ht="43" thickBot="1">
+        <v>84</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="25"/>
       <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="25"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="20"/>
-    </row>
-    <row r="13" spans="1:5" ht="28">
-      <c r="A13" s="23" t="s">
+      <c r="D12" s="27"/>
+      <c r="E12" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:5" ht="29" thickBot="1">
+    <row r="14" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25"/>
       <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="25"/>
-      <c r="D14" s="28"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="20"/>
     </row>
-    <row r="15" spans="1:5" ht="126">
-      <c r="A15" s="23" t="s">
+    <row r="15" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+      <c r="A15" s="24" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="24" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="26"/>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" spans="1:5" ht="28">
-      <c r="A16" s="24"/>
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="28"/>
       <c r="B16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="19"/>
-    </row>
-    <row r="17" spans="1:5" ht="42">
-      <c r="A17" s="24"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="31"/>
+    </row>
+    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="28"/>
       <c r="B17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:5" ht="43" thickBot="1">
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="31"/>
+    </row>
+    <row r="18" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="25"/>
       <c r="B18" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="25"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="20"/>
-    </row>
-    <row r="19" spans="1:5" ht="29" thickBot="1">
+      <c r="D18" s="27"/>
+      <c r="E18" s="32"/>
+    </row>
+    <row r="19" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
@@ -1584,93 +1632,99 @@
         <v>18</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A20" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="18"/>
-    </row>
-    <row r="21" spans="1:5" ht="29" thickBot="1">
+        <v>82</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="25"/>
       <c r="B21" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="25"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="20"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="23" t="s">
+      <c r="D21" s="27"/>
+      <c r="E21" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="24"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="28"/>
       <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="19"/>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="24"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="28"/>
       <c r="B24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="19"/>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="24"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="28"/>
       <c r="B25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="24"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="28"/>
       <c r="B26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="19"/>
     </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1">
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="25"/>
       <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="25"/>
-      <c r="D27" s="28"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="20"/>
     </row>
-    <row r="28" spans="1:5" ht="71" thickBot="1">
+    <row r="28" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -1681,11 +1735,13 @@
         <v>18</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="13"/>
-    </row>
-    <row r="29" spans="1:5" ht="29" thickBot="1">
+        <v>89</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>39</v>
       </c>
@@ -1696,11 +1752,13 @@
         <v>8</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E29" s="13"/>
-    </row>
-    <row r="30" spans="1:5" ht="29" thickBot="1">
+        <v>82</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>39</v>
       </c>
@@ -1711,11 +1769,13 @@
         <v>8</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="13"/>
-    </row>
-    <row r="31" spans="1:5" ht="29" thickBot="1">
+        <v>82</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
@@ -1726,11 +1786,13 @@
         <v>18</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="1:5" ht="29" thickBot="1">
+        <v>88</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>39</v>
       </c>
@@ -1741,11 +1803,13 @@
         <v>18</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="1:5" ht="43" thickBot="1">
+        <v>83</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>44</v>
       </c>
@@ -1756,12 +1820,14 @@
         <v>18</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33" s="13"/>
-    </row>
-    <row r="34" spans="1:5" ht="28">
-      <c r="A34" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="24" t="s">
         <v>44</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -1771,42 +1837,46 @@
         <v>49</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" s="18"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="24"/>
+        <v>82</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="28"/>
       <c r="B35" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="19"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="24"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="28"/>
       <c r="B36" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="19"/>
-    </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1">
+      <c r="D36" s="29"/>
+      <c r="E36" s="35"/>
+    </row>
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="25"/>
       <c r="B37" s="8"/>
       <c r="C37" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="28"/>
-      <c r="E37" s="20"/>
-    </row>
-    <row r="38" spans="1:5" ht="29" thickBot="1">
+      <c r="D37" s="27"/>
+      <c r="E37" s="36"/>
+    </row>
+    <row r="38" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>52</v>
       </c>
@@ -1817,26 +1887,30 @@
         <v>54</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39" spans="1:5" ht="29" thickBot="1">
+        <v>82</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="21" t="s">
         <v>56</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1">
+        <v>87</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="s">
         <v>57</v>
       </c>
@@ -1847,218 +1921,249 @@
         <v>8</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E40" s="13"/>
-    </row>
-    <row r="41" spans="1:5" ht="28">
-      <c r="A41" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="24" t="s">
         <v>59</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" s="18"/>
-    </row>
-    <row r="42" spans="1:5" ht="42">
-      <c r="A42" s="24"/>
+        <v>83</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="28"/>
       <c r="B42" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="19"/>
-    </row>
-    <row r="43" spans="1:5" ht="43" thickBot="1">
+      <c r="C42" s="28"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="25"/>
       <c r="B43" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C43" s="25"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="20"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="23" t="s">
+      <c r="D43" s="27"/>
+      <c r="E43" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="24" t="s">
         <v>59</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="23" t="s">
+      <c r="C44" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E44" s="18"/>
     </row>
-    <row r="45" spans="1:5" ht="28">
-      <c r="A45" s="24"/>
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="28"/>
       <c r="B45" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="19"/>
-    </row>
-    <row r="46" spans="1:5" ht="28">
-      <c r="A46" s="24"/>
+        <v>86</v>
+      </c>
+      <c r="C45" s="28"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="28"/>
       <c r="B46" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="24"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="19"/>
-    </row>
-    <row r="47" spans="1:5" ht="15" thickBot="1">
+      <c r="C46" s="28"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="25"/>
       <c r="B47" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C47" s="25"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="20"/>
-    </row>
-    <row r="48" spans="1:5" ht="15" thickBot="1">
+      <c r="D47" s="27"/>
+      <c r="E47" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E48" s="14"/>
-    </row>
-    <row r="49" spans="1:1">
+        <v>82</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="1" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="1" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="1" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="1" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="1" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="1" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="1" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A88" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="16">
-      <c r="A62" s="9" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="1" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="1" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="1" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A94" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="16">
-      <c r="A68" s="9" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="1"/>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
+  <mergeCells count="34">
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="C11:C12"/>
@@ -2066,33 +2171,12 @@
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E27"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2113,104 +2197,104 @@
       <selection sqref="A1:T21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="16">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="16">
-      <c r="A16" s="9" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
     </row>
   </sheetData>

</xml_diff>